<commit_message>
Re-added sleeve bearing for tonearm; includes tonearm rod updates
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8039143D-A6A9-4DDF-8369-8332189C7739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F87B868-6DA5-4292-BF50-F465466EB50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
   <si>
     <t>Part Name/URL</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>[ Details to come ]</t>
+  </si>
+  <si>
+    <t>High-Temperature Dry-Running 841 Bronze Sleeve Bearing</t>
+  </si>
+  <si>
+    <t>for 3/16" Shaft Diameter and 1/4" Housing ID, 1/4" Long</t>
   </si>
 </sst>
 </file>
@@ -652,16 +658,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFF984-406E-40B0-9A76-B0CF181B9A37}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.28515625" customWidth="1"/>
-    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" style="3" customWidth="1"/>
@@ -766,7 +772,7 @@
       </c>
       <c r="J4" s="5">
         <f>SUM(F:F)</f>
-        <v>439.76</v>
+        <v>440.37</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1509,6 +1515,23 @@
       </c>
       <c r="G42" s="6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1553,8 +1576,9 @@
     <hyperlink ref="A39" r:id="rId38" xr:uid="{BEA5C90D-4828-4877-8CED-76D896634F61}"/>
     <hyperlink ref="A41" r:id="rId39" xr:uid="{312B116C-2D5F-4265-9413-EA9A4EFC773E}"/>
     <hyperlink ref="A42" r:id="rId40" xr:uid="{BBEFB0EB-6635-402F-8279-A218F7AAAA00}"/>
+    <hyperlink ref="A43" r:id="rId41" xr:uid="{6A4C2A30-E829-4BBF-AB3B-22342EB906B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId41"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added shock-absorbant feet to parts list
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4EE1EF-D586-497C-8566-19D2E8E7A527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEE2C97-8FBB-4F29-BF4D-A7C1FDE38C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
   <si>
     <t>Part Name/URL</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Remaining Qty.</t>
   </si>
   <si>
-    <t>2 (sets)</t>
-  </si>
-  <si>
     <t>Details</t>
   </si>
   <si>
@@ -272,6 +269,9 @@
   </si>
   <si>
     <t>for 3/16" Shaft Diameter and 1/4" Housing ID, 1/4" Long</t>
+  </si>
+  <si>
+    <t>Isolation Feet</t>
   </si>
 </sst>
 </file>
@@ -658,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFF984-406E-40B0-9A76-B0CF181B9A37}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>7</v>
@@ -700,7 +700,7 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -729,14 +729,14 @@
         <v>5</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="3">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
+      <c r="D3" s="3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3</v>
       </c>
       <c r="F3" s="1">
         <v>9.99</v>
@@ -747,10 +747,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="3">
         <v>50</v>
@@ -765,160 +765,160 @@
         <v>11.8</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" s="5">
         <f>SUM(F:F)</f>
-        <v>441.59</v>
+        <v>455.78999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="3">
         <v>100</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="F5" s="1">
         <v>10.63</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
       </c>
       <c r="C6" s="3">
         <v>100</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="F6" s="1">
         <v>13.4</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
         <v>100</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F7" s="1">
         <v>10.46</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
       </c>
       <c r="C8" s="3">
         <v>100</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="F8" s="1">
         <v>7.13</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
       </c>
       <c r="C9" s="3">
         <v>100</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="F9" s="1">
         <v>5.86</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
       </c>
       <c r="C10" s="3">
         <v>100</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F10" s="1">
         <v>2.73</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -933,15 +933,15 @@
         <v>4.37</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -956,18 +956,18 @@
         <v>0.63</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3">
         <v>25</v>
@@ -982,15 +982,15 @@
         <v>8.68</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -1005,15 +1005,15 @@
         <v>23</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="3">
         <v>10</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="3">
         <v>10</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="3">
         <v>10</v>
@@ -1073,10 +1073,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>4</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" s="1">
         <v>14.69</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
@@ -1110,12 +1110,12 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="3">
         <v>25</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="3">
         <v>25</v>
@@ -1155,10 +1155,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>4</v>
@@ -1166,7 +1166,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>6</v>
@@ -1192,7 +1192,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F25" s="1">
         <v>4.2300000000000004</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="3">
         <v>4</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="3">
         <v>25</v>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="3">
         <v>20</v>
@@ -1283,10 +1283,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
         <v>58</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
       </c>
       <c r="C30" s="3">
         <v>1</v>
@@ -1306,10 +1306,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="3">
         <v>100</v>
@@ -1324,12 +1324,12 @@
         <v>8.65</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="3">
         <v>50</v>
@@ -1344,15 +1344,15 @@
         <v>8.27</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" t="s">
         <v>61</v>
-      </c>
-      <c r="B33" t="s">
-        <v>62</v>
       </c>
       <c r="C33" s="3">
         <v>50</v>
@@ -1367,12 +1367,12 @@
         <v>10.16</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="3">
         <v>5</v>
@@ -1390,15 +1390,15 @@
         <v>4</v>
       </c>
       <c r="H34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" t="s">
         <v>65</v>
-      </c>
-      <c r="B35" t="s">
-        <v>66</v>
       </c>
       <c r="D35" s="3">
         <v>2</v>
@@ -1407,12 +1407,12 @@
         <v>12.3</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="6">
         <v>858</v>
@@ -1424,15 +1424,15 @@
         <v>9.9</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" t="s">
         <v>69</v>
-      </c>
-      <c r="B37" t="s">
-        <v>70</v>
       </c>
       <c r="D37" s="3">
         <v>1</v>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D38" s="3">
         <v>4</v>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="3">
         <v>3</v>
@@ -1480,10 +1480,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F40" s="1">
         <v>13.99</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F41" s="1">
         <v>10.99</v>
@@ -1503,12 +1503,12 @@
         <v>4</v>
       </c>
       <c r="H41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F42" s="1">
         <v>6.99</v>
@@ -1519,10 +1519,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" t="s">
         <v>77</v>
-      </c>
-      <c r="B43" t="s">
-        <v>78</v>
       </c>
       <c r="D43" s="3">
         <v>3</v>
@@ -1532,7 +1532,27 @@
         <v>1.83</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="3">
+        <v>4</v>
+      </c>
+      <c r="D44" s="3">
+        <v>4</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1578,8 +1598,9 @@
     <hyperlink ref="A41" r:id="rId39" xr:uid="{312B116C-2D5F-4265-9413-EA9A4EFC773E}"/>
     <hyperlink ref="A42" r:id="rId40" xr:uid="{BBEFB0EB-6635-402F-8279-A218F7AAAA00}"/>
     <hyperlink ref="A43" r:id="rId41" xr:uid="{6A4C2A30-E829-4BBF-AB3B-22342EB906B0}"/>
+    <hyperlink ref="A44" r:id="rId42" xr:uid="{2E46890A-5D0A-4A55-9352-0ED0800B2E7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId42"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added USB cord to parts list
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEE2C97-8FBB-4F29-BF4D-A7C1FDE38C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA2092D-B177-408B-9BB8-53CF9C851FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
   <si>
     <t>Part Name/URL</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Isolation Feet</t>
+  </si>
+  <si>
+    <t>Micro USB B Male to USB B Female</t>
   </si>
 </sst>
 </file>
@@ -658,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFF984-406E-40B0-9A76-B0CF181B9A37}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +775,7 @@
       </c>
       <c r="J4" s="5">
         <f>SUM(F:F)</f>
-        <v>455.78999999999996</v>
+        <v>463.36999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1552,6 +1555,26 @@
         <v>14.2</v>
       </c>
       <c r="G44" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="3">
+        <v>1</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1">
+        <v>7.58</v>
+      </c>
+      <c r="G45" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1599,8 +1622,9 @@
     <hyperlink ref="A42" r:id="rId40" xr:uid="{BBEFB0EB-6635-402F-8279-A218F7AAAA00}"/>
     <hyperlink ref="A43" r:id="rId41" xr:uid="{6A4C2A30-E829-4BBF-AB3B-22342EB906B0}"/>
     <hyperlink ref="A44" r:id="rId42" xr:uid="{2E46890A-5D0A-4A55-9352-0ED0800B2E7E}"/>
+    <hyperlink ref="A45" r:id="rId43" xr:uid="{6359A94C-E108-400B-9B0C-E90D5B3F3C1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId43"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added rubber feet and belts to parts
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA2092D-B177-408B-9BB8-53CF9C851FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AAD0F9-E6F6-427E-B560-04D970F73CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
   <si>
     <t>Part Name/URL</t>
   </si>
@@ -253,18 +253,12 @@
     <t>LEDs</t>
   </si>
   <si>
-    <t>Custom Turntable Belts</t>
-  </si>
-  <si>
     <t>2370 Tinted Plexiglass</t>
   </si>
   <si>
     <t>Heat shrink tubing</t>
   </si>
   <si>
-    <t>[ Details to come ]</t>
-  </si>
-  <si>
     <t>High-Temperature Dry-Running 841 Bronze Sleeve Bearing</t>
   </si>
   <si>
@@ -275,6 +269,21 @@
   </si>
   <si>
     <t>Micro USB B Male to USB B Female</t>
+  </si>
+  <si>
+    <t>Custom Turntable Belt</t>
+  </si>
+  <si>
+    <t>~390mm circumference (measured from belt)</t>
+  </si>
+  <si>
+    <t>~210mm circumference (measured from belt)</t>
+  </si>
+  <si>
+    <t>Rubber Feet</t>
+  </si>
+  <si>
+    <t>1" diameter</t>
   </si>
 </sst>
 </file>
@@ -344,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -661,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFF984-406E-40B0-9A76-B0CF181B9A37}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +784,7 @@
       </c>
       <c r="J4" s="5">
         <f>SUM(F:F)</f>
-        <v>463.36999999999995</v>
+        <v>449.37999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1482,99 +1491,127 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>72</v>
+      <c r="A40" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
-      </c>
-      <c r="F40" s="1">
-        <v>13.99</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>4</v>
+        <v>79</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F41" s="1">
-        <v>10.99</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" t="s">
-        <v>35</v>
+      <c r="A41" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F42" s="1">
-        <v>6.99</v>
+        <v>10.99</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="H42" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" t="s">
-        <v>77</v>
-      </c>
-      <c r="D43" s="3">
+        <v>73</v>
+      </c>
+      <c r="F43" s="1">
+        <v>6.99</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="3">
         <v>3</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F44" s="1">
         <f>0.61*3</f>
         <v>1.83</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" s="3">
-        <v>4</v>
-      </c>
-      <c r="D44" s="3">
-        <v>4</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0</v>
-      </c>
-      <c r="F44" s="1">
-        <v>14.2</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C45" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D45" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E45" s="3">
         <v>0</v>
       </c>
       <c r="F45" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="3">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
         <v>7.58</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="G46" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="3">
+        <v>4</v>
+      </c>
+      <c r="D47" s="3">
+        <v>4</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
+      </c>
+      <c r="G47" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1618,13 +1655,15 @@
     <hyperlink ref="A37" r:id="rId36" xr:uid="{A4A22F23-99EF-42A7-B428-6D040224EB6A}"/>
     <hyperlink ref="A38" r:id="rId37" xr:uid="{8AE81F67-DB24-43CE-9063-D69E22413A0E}"/>
     <hyperlink ref="A39" r:id="rId38" xr:uid="{BEA5C90D-4828-4877-8CED-76D896634F61}"/>
-    <hyperlink ref="A41" r:id="rId39" xr:uid="{312B116C-2D5F-4265-9413-EA9A4EFC773E}"/>
-    <hyperlink ref="A42" r:id="rId40" xr:uid="{BBEFB0EB-6635-402F-8279-A218F7AAAA00}"/>
-    <hyperlink ref="A43" r:id="rId41" xr:uid="{6A4C2A30-E829-4BBF-AB3B-22342EB906B0}"/>
-    <hyperlink ref="A44" r:id="rId42" xr:uid="{2E46890A-5D0A-4A55-9352-0ED0800B2E7E}"/>
-    <hyperlink ref="A45" r:id="rId43" xr:uid="{6359A94C-E108-400B-9B0C-E90D5B3F3C1B}"/>
+    <hyperlink ref="A42" r:id="rId39" xr:uid="{312B116C-2D5F-4265-9413-EA9A4EFC773E}"/>
+    <hyperlink ref="A43" r:id="rId40" xr:uid="{BBEFB0EB-6635-402F-8279-A218F7AAAA00}"/>
+    <hyperlink ref="A44" r:id="rId41" xr:uid="{6A4C2A30-E829-4BBF-AB3B-22342EB906B0}"/>
+    <hyperlink ref="A45" r:id="rId42" xr:uid="{2E46890A-5D0A-4A55-9352-0ED0800B2E7E}"/>
+    <hyperlink ref="A46" r:id="rId43" xr:uid="{6359A94C-E108-400B-9B0C-E90D5B3F3C1B}"/>
+    <hyperlink ref="A40:A41" r:id="rId44" display="Custom Turntable Belt" xr:uid="{6D08C068-4290-4DD5-8FFF-9B40613343CF}"/>
+    <hyperlink ref="A47" r:id="rId45" xr:uid="{63E9832E-BD09-42DE-A48F-2E50997880A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId44"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Horizontal Movement Version 3 - Solenoid now directly pushes motor
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AA3A5A-AA40-4523-91B6-9E49273C1306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BC00BF-6F7B-46C4-BFF6-9FC46A692735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
   </bookViews>
@@ -277,9 +277,6 @@
     <t>5000 ohm potentiometer</t>
   </si>
   <si>
-    <t>Rubber band</t>
-  </si>
-  <si>
     <t>Ultra-Formable 260 Brass Round Tube</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>Must cut down to approx. 101mm</t>
+  </si>
+  <si>
+    <t>Music Wire Steel Extension Spring with Loop Ends</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +787,7 @@
       </c>
       <c r="J4" s="5">
         <f>SUM(F:F)</f>
-        <v>536.67000000000007</v>
+        <v>534.40000000000009</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -930,10 +930,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
         <v>81</v>
-      </c>
-      <c r="B11" t="s">
-        <v>82</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -951,7 +951,7 @@
         <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1605,22 +1605,22 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C48" s="3">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="D48" s="3">
         <v>1</v>
       </c>
       <c r="E48" s="3">
-        <v>599</v>
+        <v>0</v>
       </c>
       <c r="F48" s="1">
-        <v>5.99</v>
+        <v>3.72</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1669,8 +1669,8 @@
     <hyperlink ref="A47" r:id="rId42" xr:uid="{A8150E65-22AA-4B8C-B0A9-F8062806E414}"/>
     <hyperlink ref="A34" r:id="rId43" display="500 ohm pot" xr:uid="{1DBD9A7E-84BC-40F6-8C89-ED002140E7C3}"/>
     <hyperlink ref="A35" r:id="rId44" display="5000 ohm pot" xr:uid="{528C0C13-22D6-4D98-BBC5-98BF2F8BF63E}"/>
-    <hyperlink ref="A48" r:id="rId45" xr:uid="{4DDF16F3-DF7F-47FD-89DE-023A8C108720}"/>
-    <hyperlink ref="A11" r:id="rId46" xr:uid="{73E346AF-CF78-462D-A1B5-06E16522D199}"/>
+    <hyperlink ref="A11" r:id="rId45" xr:uid="{73E346AF-CF78-462D-A1B5-06E16522D199}"/>
+    <hyperlink ref="A48" r:id="rId46" xr:uid="{1571022E-A4EC-4606-93AC-70487020AE3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId47"/>

</xml_diff>

<commit_message>
Update parts list to reflect currently-needed parts
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82E4F8B-6B3B-4C44-9B56-C336B95BEF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A365F9D0-A34F-444E-81DA-B7E6B7200C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
   <si>
     <t>Part Name/URL</t>
   </si>
@@ -130,12 +130,6 @@
     <t>Rotary Shaft</t>
   </si>
   <si>
-    <t>1018-1045 Carbon Steel Machine Key Stock</t>
-  </si>
-  <si>
-    <t>1/8" x 1/8", 12" Long, Undersized</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -178,9 +172,6 @@
     <t>8 Pins 2.54mm Socket for Flat Ribbon Cable</t>
   </si>
   <si>
-    <t>2.54mm Male and Female Pin Headers</t>
-  </si>
-  <si>
     <t xml:space="preserve">Audio-Technica AT-VM95C Cartridge </t>
   </si>
   <si>
@@ -199,24 +190,9 @@
     <t>Cherry MX Blue Key switch</t>
   </si>
   <si>
-    <t>18-8 Stainless Steel Extra-Wide Truss Head Phillips Screws</t>
-  </si>
-  <si>
-    <t>Potentiometer knob</t>
-  </si>
-  <si>
-    <t>The higher the diameter, the easier it will be to adjust speed</t>
-  </si>
-  <si>
-    <t>DigiKey</t>
-  </si>
-  <si>
     <t>Mean Well 12v Power Supply</t>
   </si>
   <si>
-    <t>10g Calibration Weights</t>
-  </si>
-  <si>
     <t>LEDs</t>
   </si>
   <si>
@@ -241,27 +217,9 @@
     <t>Custom Turntable Belt</t>
   </si>
   <si>
-    <t>~390mm circumference (measured from belt)</t>
-  </si>
-  <si>
-    <t>~210mm circumference (measured from belt)</t>
-  </si>
-  <si>
-    <t>Rubber Feet</t>
-  </si>
-  <si>
-    <t>1" diameter</t>
-  </si>
-  <si>
     <t>Rubber bushings for motor mount</t>
   </si>
   <si>
-    <t>500 ohm potentiometer</t>
-  </si>
-  <si>
-    <t>5000 ohm potentiometer</t>
-  </si>
-  <si>
     <t>Ultra-Formable 260 Brass Round Tube</t>
   </si>
   <si>
@@ -305,6 +263,15 @@
   </si>
   <si>
     <t>5v Stepper Motor set w/ IC</t>
+  </si>
+  <si>
+    <t>~??? circumference (measured from belt)</t>
+  </si>
+  <si>
+    <t>TODO: Price is not exact</t>
+  </si>
+  <si>
+    <t>6.3v AC Transformer</t>
   </si>
 </sst>
 </file>
@@ -360,7 +327,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
@@ -375,6 +342,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -691,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFF984-406E-40B0-9A76-B0CF181B9A37}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +701,7 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -789,10 +757,10 @@
         <v>50</v>
       </c>
       <c r="D4" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F4" s="1">
         <v>11.8</v>
@@ -805,7 +773,7 @@
       </c>
       <c r="J4" s="5">
         <f>SUM(F:F)</f>
-        <v>715.26000000000033</v>
+        <v>619.09</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -948,10 +916,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -969,99 +937,93 @@
         <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
       </c>
       <c r="E12" s="3">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1">
-        <v>0.63</v>
+        <v>8.68</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H12" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
       </c>
       <c r="E13" s="3">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>8.68</v>
+        <v>25.53</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D14" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F14" s="1">
-        <v>23</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3">
         <v>10</v>
       </c>
       <c r="D15" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E15" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F15" s="1">
-        <v>9.9499999999999993</v>
+        <v>7.99</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>4</v>
@@ -1069,140 +1031,152 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3">
         <v>10</v>
       </c>
       <c r="D16" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F16" s="1">
-        <v>7.99</v>
+        <v>6.99</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="1">
+        <v>11.99</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="3">
-        <v>10</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3">
-        <v>9</v>
-      </c>
-      <c r="F17" s="1">
-        <v>6.99</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="F18" s="1">
-        <v>11.99</v>
+        <v>14.69</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
       <c r="F19" s="1">
-        <v>14.69</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="3">
+        <v>25</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>23</v>
+      </c>
+      <c r="F20" s="1">
+        <v>10.75</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C21" s="3">
         <v>25</v>
       </c>
       <c r="D21" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E21" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1">
-        <v>10.75</v>
+        <v>10.95</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>39</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="3">
-        <v>25</v>
-      </c>
-      <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3">
-        <v>24</v>
-      </c>
-      <c r="F22" s="1">
-        <v>10.95</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="C23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F23" s="1">
-        <v>5.99</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
@@ -1211,229 +1185,232 @@
         <v>0</v>
       </c>
       <c r="F24" s="1">
-        <v>39</v>
+        <v>29.99</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="3">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>7.49</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="C26" s="3">
+        <v>25</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3">
+        <v>23</v>
+      </c>
+      <c r="F26" s="1">
+        <v>6.99</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F25" s="1">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="3">
-        <v>1</v>
-      </c>
-      <c r="D26" s="3">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0</v>
-      </c>
-      <c r="F26" s="1">
-        <v>32.99</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="C27" s="3">
+        <v>20</v>
+      </c>
+      <c r="D27" s="3">
+        <v>3</v>
+      </c>
+      <c r="E27" s="3">
+        <v>17</v>
+      </c>
+      <c r="F27" s="1">
+        <v>11.99</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="1">
+        <v>11.97</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>9.99</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="3">
-        <v>4</v>
-      </c>
-      <c r="D27" s="3">
-        <v>1</v>
-      </c>
-      <c r="E27" s="3">
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>14.47</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="3">
         <v>3</v>
       </c>
-      <c r="F27" s="1">
-        <v>7.49</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="3">
-        <v>25</v>
-      </c>
-      <c r="D28" s="3">
-        <v>2</v>
-      </c>
-      <c r="E28" s="3">
-        <v>23</v>
-      </c>
-      <c r="F28" s="1">
-        <v>6.99</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="3">
-        <v>20</v>
-      </c>
-      <c r="D29" s="3">
-        <v>3</v>
-      </c>
-      <c r="E29" s="3">
-        <v>17</v>
-      </c>
-      <c r="F29" s="1">
-        <v>11.99</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="3">
-        <v>100</v>
-      </c>
       <c r="D31" s="3">
-        <v>6</v>
+        <v>600</v>
       </c>
       <c r="E31" s="3">
-        <v>94</v>
+        <v>597</v>
       </c>
       <c r="F31" s="1">
-        <v>8.65</v>
+        <v>12.99</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>72</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
       </c>
       <c r="F32" s="1">
-        <v>11.97</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>4</v>
+        <v>35</v>
+      </c>
+      <c r="H32" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="3">
-        <v>5</v>
-      </c>
-      <c r="D33" s="3">
-        <v>2</v>
-      </c>
-      <c r="E33" s="3">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="F33" s="1">
-        <v>13.99</v>
+        <v>10.99</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="3">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="F34" s="1">
-        <v>1.72</v>
+        <v>6.99</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>74</v>
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
       </c>
       <c r="D35" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F35" s="1">
-        <v>1.72</v>
+        <f>0.67*5</f>
+        <v>3.35</v>
       </c>
       <c r="G35" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>88</v>
+      <c r="C36" s="3">
+        <v>4</v>
       </c>
       <c r="D36" s="3">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
       </c>
       <c r="F36" s="1">
-        <v>9.99</v>
+        <v>14.2</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B37" t="s">
-        <v>78</v>
+      <c r="C37" s="3">
+        <v>1</v>
       </c>
       <c r="D37" s="3">
         <v>1</v>
       </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
       <c r="F37" s="1">
-        <v>14.47</v>
+        <v>7.58</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>4</v>
@@ -1441,13 +1418,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D38" s="3">
-        <v>4</v>
+        <v>67</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
       </c>
       <c r="F38" s="1">
-        <v>21.96</v>
+        <v>13.99</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>4</v>
@@ -1455,19 +1432,19 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C39" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D39" s="3">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="E39" s="3">
-        <v>597</v>
+        <v>4</v>
       </c>
       <c r="F39" s="1">
-        <v>12.99</v>
+        <v>14.99</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>4</v>
@@ -1475,207 +1452,56 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
       </c>
       <c r="D40" s="3">
         <v>1</v>
       </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
       <c r="F40" s="1">
-        <v>36.450000000000003</v>
+        <v>132.22</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>67</v>
+      <c r="A41" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D41" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41" s="1">
-        <v>36.450000000000003</v>
+        <v>7.26</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>61</v>
+        <v>78</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
       </c>
       <c r="F42" s="1">
-        <v>10.99</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H42" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F43" s="1">
-        <v>6.99</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="3">
-        <v>5</v>
-      </c>
-      <c r="F44" s="1">
-        <f>0.67*5</f>
-        <v>3.35</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="3">
-        <v>4</v>
-      </c>
-      <c r="D45" s="3">
-        <v>4</v>
-      </c>
-      <c r="E45" s="3">
-        <v>0</v>
-      </c>
-      <c r="F45" s="1">
-        <v>14.2</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="3">
-        <v>1</v>
-      </c>
-      <c r="D46" s="3">
-        <v>1</v>
-      </c>
-      <c r="E46" s="3">
-        <v>0</v>
-      </c>
-      <c r="F46" s="1">
-        <v>7.58</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C47" s="3">
-        <v>4</v>
-      </c>
-      <c r="D47" s="3">
-        <v>4</v>
-      </c>
-      <c r="E47" s="3">
-        <v>0</v>
-      </c>
-      <c r="F47" s="1">
-        <v>14.2</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B48" t="s">
-        <v>82</v>
-      </c>
-      <c r="F48" s="1">
-        <v>13.99</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="3">
-        <v>5</v>
-      </c>
-      <c r="D49" s="3">
-        <v>1</v>
-      </c>
-      <c r="E49" s="3">
-        <v>4</v>
-      </c>
-      <c r="F49" s="1">
-        <v>14.99</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="3">
-        <v>1</v>
-      </c>
-      <c r="D50" s="3">
-        <v>1</v>
-      </c>
-      <c r="E50" s="3">
-        <v>0</v>
-      </c>
-      <c r="F50" s="1">
-        <v>132.22</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B51" t="s">
-        <v>87</v>
-      </c>
-      <c r="D51" s="3">
-        <v>2</v>
-      </c>
-      <c r="F51" s="1">
-        <v>7.26</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>13</v>
+        <v>11.06</v>
       </c>
     </row>
   </sheetData>
@@ -1689,47 +1515,39 @@
     <hyperlink ref="A8" r:id="rId7" xr:uid="{9BCD095B-47DC-410F-9079-F7EF1073AAB6}"/>
     <hyperlink ref="A9" r:id="rId8" xr:uid="{602A26C0-072C-4CA0-B060-8605A9A79C99}"/>
     <hyperlink ref="A10" r:id="rId9" xr:uid="{CB2F58B0-3E1A-45F1-9BAF-84747E9E2286}"/>
-    <hyperlink ref="A12" r:id="rId10" xr:uid="{1128674C-B084-46B4-B266-A27FCB34E55D}"/>
-    <hyperlink ref="A13" r:id="rId11" xr:uid="{3248FF67-9F07-4CAC-8A23-E7D040BAF240}"/>
-    <hyperlink ref="A14" r:id="rId12" xr:uid="{036623F6-4A17-4DC1-B412-5D2B9F531304}"/>
-    <hyperlink ref="A15" r:id="rId13" xr:uid="{FE7980E9-66C7-4203-A284-299B9289A69F}"/>
-    <hyperlink ref="A16" r:id="rId14" xr:uid="{919D209F-D950-4910-849B-5AB77A6C3FE8}"/>
-    <hyperlink ref="A17" r:id="rId15" xr:uid="{B39BD6B0-9D3E-4F4D-9289-008736E9AB9E}"/>
-    <hyperlink ref="A18" r:id="rId16" xr:uid="{DC2AB890-168C-4E32-A4B1-D4FE8EFB056E}"/>
-    <hyperlink ref="A19" r:id="rId17" xr:uid="{3B9AA3BB-A878-47F5-8FD7-E001F7473C4C}"/>
-    <hyperlink ref="A20" r:id="rId18" xr:uid="{DAA1FD29-C47C-42D3-A904-F870B4A44071}"/>
-    <hyperlink ref="A21" r:id="rId19" xr:uid="{71194D6C-4C2C-40AE-BA02-4EE66C79B901}"/>
-    <hyperlink ref="A22" r:id="rId20" xr:uid="{06D49833-6463-4404-A46B-44C35596620D}"/>
-    <hyperlink ref="A23" r:id="rId21" xr:uid="{804ABA83-E1BC-4E17-9411-09F4CAFAA514}"/>
-    <hyperlink ref="A24" r:id="rId22" xr:uid="{49D42AB6-4BE9-4066-8807-9A44A8AE697C}"/>
-    <hyperlink ref="A25" r:id="rId23" xr:uid="{D39B49A4-0862-4B0C-A68D-D8A021F9D2A2}"/>
-    <hyperlink ref="A27" r:id="rId24" xr:uid="{CFEE09BC-B295-4BB1-A6E5-DC54B1C602CC}"/>
-    <hyperlink ref="A28" r:id="rId25" xr:uid="{D1AF1FD1-DBE3-4AF5-A0AF-E7534826D87A}"/>
-    <hyperlink ref="A29" r:id="rId26" xr:uid="{C84E2B92-5A19-4D83-8C00-11FF9D3EB587}"/>
-    <hyperlink ref="A31" r:id="rId27" xr:uid="{244C681C-B938-4F5B-BCCB-2516999BBB91}"/>
-    <hyperlink ref="A33" r:id="rId28" xr:uid="{DD3340E7-A316-4150-B333-5B6608C8820E}"/>
-    <hyperlink ref="A38" r:id="rId29" xr:uid="{8AE81F67-DB24-43CE-9063-D69E22413A0E}"/>
-    <hyperlink ref="A39" r:id="rId30" xr:uid="{BEA5C90D-4828-4877-8CED-76D896634F61}"/>
-    <hyperlink ref="A42" r:id="rId31" xr:uid="{312B116C-2D5F-4265-9413-EA9A4EFC773E}"/>
-    <hyperlink ref="A43" r:id="rId32" xr:uid="{BBEFB0EB-6635-402F-8279-A218F7AAAA00}"/>
-    <hyperlink ref="A44" r:id="rId33" xr:uid="{6A4C2A30-E829-4BBF-AB3B-22342EB906B0}"/>
-    <hyperlink ref="A45" r:id="rId34" xr:uid="{2E46890A-5D0A-4A55-9352-0ED0800B2E7E}"/>
-    <hyperlink ref="A46" r:id="rId35" xr:uid="{6359A94C-E108-400B-9B0C-E90D5B3F3C1B}"/>
-    <hyperlink ref="A40:A41" r:id="rId36" display="Custom Turntable Belt" xr:uid="{6D08C068-4290-4DD5-8FFF-9B40613343CF}"/>
-    <hyperlink ref="A32" r:id="rId37" xr:uid="{64D620F9-BE29-4078-8FDB-01AADED4CD5A}"/>
-    <hyperlink ref="A47" r:id="rId38" xr:uid="{A8150E65-22AA-4B8C-B0A9-F8062806E414}"/>
-    <hyperlink ref="A34" r:id="rId39" display="500 ohm pot" xr:uid="{1DBD9A7E-84BC-40F6-8C89-ED002140E7C3}"/>
-    <hyperlink ref="A35" r:id="rId40" display="5000 ohm pot" xr:uid="{528C0C13-22D6-4D98-BBC5-98BF2F8BF63E}"/>
-    <hyperlink ref="A11" r:id="rId41" xr:uid="{73E346AF-CF78-462D-A1B5-06E16522D199}"/>
-    <hyperlink ref="A37" r:id="rId42" xr:uid="{068F758C-56B5-4BE6-8457-882D40684EC8}"/>
-    <hyperlink ref="A26" r:id="rId43" xr:uid="{DD1952C6-DDB9-46AB-BAF6-438AD299B4B9}"/>
-    <hyperlink ref="A48" r:id="rId44" xr:uid="{8EDB4583-9C54-449A-B150-77F255495BD5}"/>
-    <hyperlink ref="A49" r:id="rId45" xr:uid="{F26BE873-0541-4AD7-B469-EEC4ECF1ACE8}"/>
-    <hyperlink ref="A50" r:id="rId46" xr:uid="{A56A6466-8646-4733-BAB4-237D1A4B7620}"/>
-    <hyperlink ref="A51" r:id="rId47" xr:uid="{081913BF-1751-47D6-B8AD-C966158B1155}"/>
-    <hyperlink ref="A36" r:id="rId48" display="Adafruit 858 Stepper Motor" xr:uid="{474E9ED2-9AFC-49D6-855D-64137217487B}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{3248FF67-9F07-4CAC-8A23-E7D040BAF240}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{036623F6-4A17-4DC1-B412-5D2B9F531304}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{FE7980E9-66C7-4203-A284-299B9289A69F}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{919D209F-D950-4910-849B-5AB77A6C3FE8}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{B39BD6B0-9D3E-4F4D-9289-008736E9AB9E}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{DC2AB890-168C-4E32-A4B1-D4FE8EFB056E}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{3B9AA3BB-A878-47F5-8FD7-E001F7473C4C}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{DAA1FD29-C47C-42D3-A904-F870B4A44071}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{71194D6C-4C2C-40AE-BA02-4EE66C79B901}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{06D49833-6463-4404-A46B-44C35596620D}"/>
+    <hyperlink ref="A22" r:id="rId20" xr:uid="{49D42AB6-4BE9-4066-8807-9A44A8AE697C}"/>
+    <hyperlink ref="A23" r:id="rId21" xr:uid="{D39B49A4-0862-4B0C-A68D-D8A021F9D2A2}"/>
+    <hyperlink ref="A25" r:id="rId22" xr:uid="{CFEE09BC-B295-4BB1-A6E5-DC54B1C602CC}"/>
+    <hyperlink ref="A26" r:id="rId23" xr:uid="{D1AF1FD1-DBE3-4AF5-A0AF-E7534826D87A}"/>
+    <hyperlink ref="A27" r:id="rId24" xr:uid="{C84E2B92-5A19-4D83-8C00-11FF9D3EB587}"/>
+    <hyperlink ref="A31" r:id="rId25" xr:uid="{BEA5C90D-4828-4877-8CED-76D896634F61}"/>
+    <hyperlink ref="A33" r:id="rId26" xr:uid="{312B116C-2D5F-4265-9413-EA9A4EFC773E}"/>
+    <hyperlink ref="A34" r:id="rId27" xr:uid="{BBEFB0EB-6635-402F-8279-A218F7AAAA00}"/>
+    <hyperlink ref="A35" r:id="rId28" xr:uid="{6A4C2A30-E829-4BBF-AB3B-22342EB906B0}"/>
+    <hyperlink ref="A36" r:id="rId29" xr:uid="{2E46890A-5D0A-4A55-9352-0ED0800B2E7E}"/>
+    <hyperlink ref="A37" r:id="rId30" xr:uid="{6359A94C-E108-400B-9B0C-E90D5B3F3C1B}"/>
+    <hyperlink ref="A28" r:id="rId31" xr:uid="{64D620F9-BE29-4078-8FDB-01AADED4CD5A}"/>
+    <hyperlink ref="A11" r:id="rId32" xr:uid="{73E346AF-CF78-462D-A1B5-06E16522D199}"/>
+    <hyperlink ref="A30" r:id="rId33" xr:uid="{068F758C-56B5-4BE6-8457-882D40684EC8}"/>
+    <hyperlink ref="A24" r:id="rId34" xr:uid="{DD1952C6-DDB9-46AB-BAF6-438AD299B4B9}"/>
+    <hyperlink ref="A38" r:id="rId35" xr:uid="{8EDB4583-9C54-449A-B150-77F255495BD5}"/>
+    <hyperlink ref="A39" r:id="rId36" xr:uid="{F26BE873-0541-4AD7-B469-EEC4ECF1ACE8}"/>
+    <hyperlink ref="A40" r:id="rId37" xr:uid="{A56A6466-8646-4733-BAB4-237D1A4B7620}"/>
+    <hyperlink ref="A41" r:id="rId38" xr:uid="{081913BF-1751-47D6-B8AD-C966158B1155}"/>
+    <hyperlink ref="A29" r:id="rId39" display="Adafruit 858 Stepper Motor" xr:uid="{474E9ED2-9AFC-49D6-855D-64137217487B}"/>
+    <hyperlink ref="A42" r:id="rId40" xr:uid="{1F56827A-8EC4-4506-A806-69B5F684DE5C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId49"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove 7-segment from parts list
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A365F9D0-A34F-444E-81DA-B7E6B7200C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EF3F3A-10EE-43B4-87F8-5EA1D6FFA60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
   <si>
     <t>Part Name/URL</t>
   </si>
@@ -158,12 +158,6 @@
   </si>
   <si>
     <t>Rainbow Ribbon Cable</t>
-  </si>
-  <si>
-    <t>Adafruit</t>
-  </si>
-  <si>
-    <t>4-Digit 7-Segment Display w/I2C Backpack</t>
   </si>
   <si>
     <t>6 Pins Dual Row Sockets for Flat Ribbon Cable</t>
@@ -327,7 +321,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
@@ -342,7 +336,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -659,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFF984-406E-40B0-9A76-B0CF181B9A37}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,7 +766,7 @@
       </c>
       <c r="J4" s="5">
         <f>SUM(F:F)</f>
-        <v>619.09</v>
+        <v>609.1400000000001</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -916,10 +909,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -937,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1017,10 +1010,10 @@
         <v>10</v>
       </c>
       <c r="D15" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F15" s="1">
         <v>7.99</v>
@@ -1073,39 +1066,39 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="3">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F19" s="1">
-        <v>9.9499999999999993</v>
+        <v>10.75</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="3">
         <v>25</v>
       </c>
       <c r="D20" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F20" s="1">
-        <v>10.75</v>
+        <v>10.95</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>4</v>
@@ -1113,19 +1106,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="3">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
       </c>
       <c r="E21" s="3">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F21" s="1">
-        <v>10.95</v>
+        <v>39</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>4</v>
@@ -1133,16 +1123,19 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
       <c r="F22" s="1">
-        <v>39</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>4</v>
@@ -1150,19 +1143,22 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>47</v>
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
       </c>
       <c r="F23" s="1">
-        <v>4.2300000000000004</v>
+        <v>29.99</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>4</v>
@@ -1170,22 +1166,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
       </c>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F24" s="1">
-        <v>29.99</v>
+        <v>7.49</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>4</v>
@@ -1193,19 +1186,19 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="3">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D25" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="3">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F25" s="1">
-        <v>7.49</v>
+        <v>6.99</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>4</v>
@@ -1213,19 +1206,19 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="3">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D26" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26" s="3">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F26" s="1">
-        <v>6.99</v>
+        <v>11.99</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>4</v>
@@ -1233,30 +1226,27 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="3">
-        <v>20</v>
-      </c>
-      <c r="D27" s="3">
-        <v>3</v>
-      </c>
-      <c r="E27" s="3">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="F27" s="1">
-        <v>11.99</v>
+        <v>11.97</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>60</v>
+      <c r="A28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2</v>
       </c>
       <c r="F28" s="1">
-        <v>11.97</v>
+        <v>9.99</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>4</v>
@@ -1264,243 +1254,226 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>14.47</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3</v>
+      </c>
+      <c r="D30" s="3">
+        <v>600</v>
+      </c>
+      <c r="E30" s="3">
+        <v>597</v>
+      </c>
+      <c r="F30" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>35</v>
+      </c>
+      <c r="H31" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="3">
-        <v>2</v>
-      </c>
-      <c r="F29" s="1">
-        <v>9.99</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="3">
-        <v>1</v>
-      </c>
-      <c r="F30" s="1">
-        <v>14.47</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="F32" s="1">
+        <v>10.99</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="3">
-        <v>3</v>
-      </c>
-      <c r="D31" s="3">
-        <v>600</v>
-      </c>
-      <c r="E31" s="3">
-        <v>597</v>
-      </c>
-      <c r="F31" s="1">
-        <v>12.99</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="3">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1">
-        <v>35</v>
-      </c>
-      <c r="H32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="F33" s="1">
+        <v>6.99</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="1">
-        <v>10.99</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B34" t="s">
         <v>54</v>
       </c>
+      <c r="D34" s="3">
+        <v>5</v>
+      </c>
       <c r="F34" s="1">
-        <v>6.99</v>
+        <f>0.67*5</f>
+        <v>3.35</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" s="3">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3">
+        <v>4</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="3">
-        <v>5</v>
-      </c>
-      <c r="F35" s="1">
-        <f>0.67*5</f>
-        <v>3.35</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="C36" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D36" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
       <c r="F36" s="1">
-        <v>14.2</v>
+        <v>7.58</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="3">
-        <v>1</v>
-      </c>
-      <c r="D37" s="3">
-        <v>1</v>
-      </c>
-      <c r="E37" s="3">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
       </c>
       <c r="F37" s="1">
-        <v>7.58</v>
+        <v>13.99</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" s="3">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3">
+        <v>4</v>
+      </c>
+      <c r="F38" s="1">
+        <v>14.99</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="1">
-        <v>13.99</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="C39" s="3">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1">
+        <v>132.22</v>
+      </c>
+      <c r="G39" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="3">
-        <v>5</v>
-      </c>
-      <c r="D39" s="3">
-        <v>1</v>
-      </c>
-      <c r="E39" s="3">
-        <v>4</v>
-      </c>
-      <c r="F39" s="1">
-        <v>14.99</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="3">
-        <v>1</v>
+      <c r="B40" t="s">
+        <v>71</v>
       </c>
       <c r="D40" s="3">
-        <v>1</v>
-      </c>
-      <c r="E40" s="3">
+        <v>2</v>
+      </c>
+      <c r="F40" s="1">
+        <v>7.26</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3">
         <v>0</v>
       </c>
-      <c r="F40" s="1">
-        <v>132.22</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" s="3">
-        <v>2</v>
-      </c>
       <c r="F41" s="1">
-        <v>7.26</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" s="3">
-        <v>1</v>
-      </c>
-      <c r="D42" s="3">
-        <v>1</v>
-      </c>
-      <c r="E42" s="3">
-        <v>0</v>
-      </c>
-      <c r="F42" s="1">
         <v>11.06</v>
       </c>
     </row>
@@ -1522,32 +1495,31 @@
     <hyperlink ref="A16" r:id="rId14" xr:uid="{B39BD6B0-9D3E-4F4D-9289-008736E9AB9E}"/>
     <hyperlink ref="A17" r:id="rId15" xr:uid="{DC2AB890-168C-4E32-A4B1-D4FE8EFB056E}"/>
     <hyperlink ref="A18" r:id="rId16" xr:uid="{3B9AA3BB-A878-47F5-8FD7-E001F7473C4C}"/>
-    <hyperlink ref="A19" r:id="rId17" xr:uid="{DAA1FD29-C47C-42D3-A904-F870B4A44071}"/>
-    <hyperlink ref="A20" r:id="rId18" xr:uid="{71194D6C-4C2C-40AE-BA02-4EE66C79B901}"/>
-    <hyperlink ref="A21" r:id="rId19" xr:uid="{06D49833-6463-4404-A46B-44C35596620D}"/>
-    <hyperlink ref="A22" r:id="rId20" xr:uid="{49D42AB6-4BE9-4066-8807-9A44A8AE697C}"/>
-    <hyperlink ref="A23" r:id="rId21" xr:uid="{D39B49A4-0862-4B0C-A68D-D8A021F9D2A2}"/>
-    <hyperlink ref="A25" r:id="rId22" xr:uid="{CFEE09BC-B295-4BB1-A6E5-DC54B1C602CC}"/>
-    <hyperlink ref="A26" r:id="rId23" xr:uid="{D1AF1FD1-DBE3-4AF5-A0AF-E7534826D87A}"/>
-    <hyperlink ref="A27" r:id="rId24" xr:uid="{C84E2B92-5A19-4D83-8C00-11FF9D3EB587}"/>
-    <hyperlink ref="A31" r:id="rId25" xr:uid="{BEA5C90D-4828-4877-8CED-76D896634F61}"/>
-    <hyperlink ref="A33" r:id="rId26" xr:uid="{312B116C-2D5F-4265-9413-EA9A4EFC773E}"/>
-    <hyperlink ref="A34" r:id="rId27" xr:uid="{BBEFB0EB-6635-402F-8279-A218F7AAAA00}"/>
-    <hyperlink ref="A35" r:id="rId28" xr:uid="{6A4C2A30-E829-4BBF-AB3B-22342EB906B0}"/>
-    <hyperlink ref="A36" r:id="rId29" xr:uid="{2E46890A-5D0A-4A55-9352-0ED0800B2E7E}"/>
-    <hyperlink ref="A37" r:id="rId30" xr:uid="{6359A94C-E108-400B-9B0C-E90D5B3F3C1B}"/>
-    <hyperlink ref="A28" r:id="rId31" xr:uid="{64D620F9-BE29-4078-8FDB-01AADED4CD5A}"/>
-    <hyperlink ref="A11" r:id="rId32" xr:uid="{73E346AF-CF78-462D-A1B5-06E16522D199}"/>
-    <hyperlink ref="A30" r:id="rId33" xr:uid="{068F758C-56B5-4BE6-8457-882D40684EC8}"/>
-    <hyperlink ref="A24" r:id="rId34" xr:uid="{DD1952C6-DDB9-46AB-BAF6-438AD299B4B9}"/>
-    <hyperlink ref="A38" r:id="rId35" xr:uid="{8EDB4583-9C54-449A-B150-77F255495BD5}"/>
-    <hyperlink ref="A39" r:id="rId36" xr:uid="{F26BE873-0541-4AD7-B469-EEC4ECF1ACE8}"/>
-    <hyperlink ref="A40" r:id="rId37" xr:uid="{A56A6466-8646-4733-BAB4-237D1A4B7620}"/>
-    <hyperlink ref="A41" r:id="rId38" xr:uid="{081913BF-1751-47D6-B8AD-C966158B1155}"/>
-    <hyperlink ref="A29" r:id="rId39" display="Adafruit 858 Stepper Motor" xr:uid="{474E9ED2-9AFC-49D6-855D-64137217487B}"/>
-    <hyperlink ref="A42" r:id="rId40" xr:uid="{1F56827A-8EC4-4506-A806-69B5F684DE5C}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{71194D6C-4C2C-40AE-BA02-4EE66C79B901}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{06D49833-6463-4404-A46B-44C35596620D}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{49D42AB6-4BE9-4066-8807-9A44A8AE697C}"/>
+    <hyperlink ref="A22" r:id="rId20" xr:uid="{D39B49A4-0862-4B0C-A68D-D8A021F9D2A2}"/>
+    <hyperlink ref="A24" r:id="rId21" xr:uid="{CFEE09BC-B295-4BB1-A6E5-DC54B1C602CC}"/>
+    <hyperlink ref="A25" r:id="rId22" xr:uid="{D1AF1FD1-DBE3-4AF5-A0AF-E7534826D87A}"/>
+    <hyperlink ref="A26" r:id="rId23" xr:uid="{C84E2B92-5A19-4D83-8C00-11FF9D3EB587}"/>
+    <hyperlink ref="A30" r:id="rId24" xr:uid="{BEA5C90D-4828-4877-8CED-76D896634F61}"/>
+    <hyperlink ref="A32" r:id="rId25" xr:uid="{312B116C-2D5F-4265-9413-EA9A4EFC773E}"/>
+    <hyperlink ref="A33" r:id="rId26" xr:uid="{BBEFB0EB-6635-402F-8279-A218F7AAAA00}"/>
+    <hyperlink ref="A34" r:id="rId27" xr:uid="{6A4C2A30-E829-4BBF-AB3B-22342EB906B0}"/>
+    <hyperlink ref="A35" r:id="rId28" xr:uid="{2E46890A-5D0A-4A55-9352-0ED0800B2E7E}"/>
+    <hyperlink ref="A36" r:id="rId29" xr:uid="{6359A94C-E108-400B-9B0C-E90D5B3F3C1B}"/>
+    <hyperlink ref="A27" r:id="rId30" xr:uid="{64D620F9-BE29-4078-8FDB-01AADED4CD5A}"/>
+    <hyperlink ref="A11" r:id="rId31" xr:uid="{73E346AF-CF78-462D-A1B5-06E16522D199}"/>
+    <hyperlink ref="A29" r:id="rId32" xr:uid="{068F758C-56B5-4BE6-8457-882D40684EC8}"/>
+    <hyperlink ref="A23" r:id="rId33" xr:uid="{DD1952C6-DDB9-46AB-BAF6-438AD299B4B9}"/>
+    <hyperlink ref="A37" r:id="rId34" xr:uid="{8EDB4583-9C54-449A-B150-77F255495BD5}"/>
+    <hyperlink ref="A38" r:id="rId35" xr:uid="{F26BE873-0541-4AD7-B469-EEC4ECF1ACE8}"/>
+    <hyperlink ref="A39" r:id="rId36" xr:uid="{A56A6466-8646-4733-BAB4-237D1A4B7620}"/>
+    <hyperlink ref="A40" r:id="rId37" xr:uid="{081913BF-1751-47D6-B8AD-C966158B1155}"/>
+    <hyperlink ref="A28" r:id="rId38" display="Adafruit 858 Stepper Motor" xr:uid="{474E9ED2-9AFC-49D6-855D-64137217487B}"/>
+    <hyperlink ref="A41" r:id="rId39" xr:uid="{1F56827A-8EC4-4506-A806-69B5F684DE5C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId41"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finish PCB 0.5 - still need to do BOM
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EF3F3A-10EE-43B4-87F8-5EA1D6FFA60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683559BB-A1D5-4FE3-AB97-A02CD1C501E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
   <si>
     <t>Part Name/URL</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>6.3v AC Transformer</t>
+  </si>
+  <si>
+    <t>Parallel port</t>
+  </si>
+  <si>
+    <t>171-025-103L001</t>
   </si>
 </sst>
 </file>
@@ -652,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFF984-406E-40B0-9A76-B0CF181B9A37}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +772,7 @@
       </c>
       <c r="J4" s="5">
         <f>SUM(F:F)</f>
-        <v>609.1400000000001</v>
+        <v>610.83000000000015</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1475,6 +1481,26 @@
       </c>
       <c r="F41" s="1">
         <v>11.06</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1.69</v>
       </c>
     </row>
   </sheetData>
@@ -1518,8 +1544,9 @@
     <hyperlink ref="A40" r:id="rId37" xr:uid="{081913BF-1751-47D6-B8AD-C966158B1155}"/>
     <hyperlink ref="A28" r:id="rId38" display="Adafruit 858 Stepper Motor" xr:uid="{474E9ED2-9AFC-49D6-855D-64137217487B}"/>
     <hyperlink ref="A41" r:id="rId39" xr:uid="{1F56827A-8EC4-4506-A806-69B5F684DE5C}"/>
+    <hyperlink ref="A42" r:id="rId40" xr:uid="{12164573-0FDC-4B10-A12A-CC40E343CC16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId40"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fit encoder on test setup - still need to transfer to movement hub
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683559BB-A1D5-4FE3-AB97-A02CD1C501E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DA3535-DB90-4626-804E-07A77A682037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
   <si>
     <t>Part Name/URL</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>171-025-103L001</t>
+  </si>
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>DigiKey</t>
   </si>
 </sst>
 </file>
@@ -658,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFF984-406E-40B0-9A76-B0CF181B9A37}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +778,7 @@
       </c>
       <c r="J4" s="5">
         <f>SUM(F:F)</f>
-        <v>610.83000000000015</v>
+        <v>626.25000000000011</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1501,6 +1507,26 @@
       </c>
       <c r="F42" s="1">
         <v>1.69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1">
+        <v>15.42</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1545,8 +1571,9 @@
     <hyperlink ref="A28" r:id="rId38" display="Adafruit 858 Stepper Motor" xr:uid="{474E9ED2-9AFC-49D6-855D-64137217487B}"/>
     <hyperlink ref="A41" r:id="rId39" xr:uid="{1F56827A-8EC4-4506-A806-69B5F684DE5C}"/>
     <hyperlink ref="A42" r:id="rId40" xr:uid="{12164573-0FDC-4B10-A12A-CC40E343CC16}"/>
+    <hyperlink ref="A43" r:id="rId41" xr:uid="{820FF4A0-CDA2-495F-8E9D-9F47FAB7A271}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId41"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Transfer encoder changes to tonearm movement hub
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DA3535-DB90-4626-804E-07A77A682037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DF7AF8-DB73-480B-B479-9B3224371038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
   <si>
     <t>Part Name/URL</t>
   </si>
@@ -278,6 +278,18 @@
   </si>
   <si>
     <t>DigiKey</t>
+  </si>
+  <si>
+    <t>Thread</t>
+  </si>
+  <si>
+    <t>Only needed for internal anti-skate; any thread will do</t>
+  </si>
+  <si>
+    <t>Music Wire Steel Extension Spring with Loop Ends</t>
+  </si>
+  <si>
+    <t>Corrosion-Resistant Curved Disc Springs</t>
   </si>
 </sst>
 </file>
@@ -664,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFF984-406E-40B0-9A76-B0CF181B9A37}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +790,7 @@
       </c>
       <c r="J4" s="5">
         <f>SUM(F:F)</f>
-        <v>626.25000000000011</v>
+        <v>661.66000000000008</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1463,10 +1475,10 @@
         <v>71</v>
       </c>
       <c r="D40" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F40" s="1">
-        <v>7.26</v>
+        <v>11.73</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>13</v>
@@ -1488,6 +1500,9 @@
       <c r="F41" s="1">
         <v>11.06</v>
       </c>
+      <c r="G41" s="6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -1508,6 +1523,9 @@
       <c r="F42" s="1">
         <v>1.69</v>
       </c>
+      <c r="G42" s="6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
@@ -1527,6 +1545,69 @@
       </c>
       <c r="G43" s="6" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="3">
+        <v>1</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>4.26</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="3">
+        <v>5</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3">
+        <v>4</v>
+      </c>
+      <c r="F45" s="1">
+        <v>14.92</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="3">
+        <v>5</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
+        <v>4</v>
+      </c>
+      <c r="F46" s="1">
+        <v>11.76</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1572,8 +1653,11 @@
     <hyperlink ref="A41" r:id="rId39" xr:uid="{1F56827A-8EC4-4506-A806-69B5F684DE5C}"/>
     <hyperlink ref="A42" r:id="rId40" xr:uid="{12164573-0FDC-4B10-A12A-CC40E343CC16}"/>
     <hyperlink ref="A43" r:id="rId41" xr:uid="{820FF4A0-CDA2-495F-8E9D-9F47FAB7A271}"/>
+    <hyperlink ref="A44" r:id="rId42" xr:uid="{C3F4C230-2C94-4F28-852B-556D69F4D837}"/>
+    <hyperlink ref="A45" r:id="rId43" xr:uid="{8D69888B-2039-4A9C-973D-8028D4E1E97C}"/>
+    <hyperlink ref="A46" r:id="rId44" xr:uid="{D16355A9-735E-4FF6-8453-810E60FD4015}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId42"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Prototype new anti-skate mechanism - still need to add to movement hub
</commit_message>
<xml_diff>
--- a/parts-list.xlsx
+++ b/parts-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DF7AF8-DB73-480B-B479-9B3224371038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906633D6-1A97-42E5-BAFF-7DC616CE72FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A06A66CB-E3E2-4981-B2CE-614E0D52BEF1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="88">
   <si>
     <t>Part Name/URL</t>
   </si>
@@ -214,15 +214,6 @@
     <t>Rubber bushings for motor mount</t>
   </si>
   <si>
-    <t>Ultra-Formable 260 Brass Round Tube</t>
-  </si>
-  <si>
-    <t>1 Foot Long, 0.049" Wall Thickness, 3/16" OD</t>
-  </si>
-  <si>
-    <t>Must cut down to approx. 101mm</t>
-  </si>
-  <si>
     <t xml:space="preserve">RS-25-12 12V 2.1 Amp </t>
   </si>
   <si>
@@ -290,6 +281,24 @@
   </si>
   <si>
     <t>Corrosion-Resistant Curved Disc Springs</t>
+  </si>
+  <si>
+    <t>Ball Bearing 3/8" shaft diameter</t>
+  </si>
+  <si>
+    <t>18-8 Stainless Steel Washer</t>
+  </si>
+  <si>
+    <t>for Number 10 Screw Size, 0.203" ID, 0.438" OD</t>
+  </si>
+  <si>
+    <t>Multipurpose 6061 Aluminum Round Tube</t>
+  </si>
+  <si>
+    <t>0.035" Wall Thickness, 3/8" OD</t>
+  </si>
+  <si>
+    <t>2ft length</t>
   </si>
 </sst>
 </file>
@@ -676,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFF984-406E-40B0-9A76-B0CF181B9A37}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,7 +799,7 @@
       </c>
       <c r="J4" s="5">
         <f>SUM(F:F)</f>
-        <v>661.66000000000008</v>
+        <v>675.67</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -933,28 +942,22 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
       </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
       <c r="F11" s="1">
-        <v>13.89</v>
+        <v>13.72</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1014,10 +1017,10 @@
         <v>10</v>
       </c>
       <c r="D14" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E14" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F14" s="1">
         <v>9.9499999999999993</v>
@@ -1167,10 +1170,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -1261,10 +1264,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D28" s="3">
         <v>2</v>
@@ -1281,7 +1284,7 @@
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -1318,7 +1321,7 @@
         <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -1327,7 +1330,7 @@
         <v>35</v>
       </c>
       <c r="H31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1415,10 +1418,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F37" s="1">
         <v>13.99</v>
@@ -1429,7 +1432,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C38" s="3">
         <v>5</v>
@@ -1449,7 +1452,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C39" s="3">
         <v>1</v>
@@ -1464,15 +1467,15 @@
         <v>132.22</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D40" s="3">
         <v>3</v>
@@ -1486,7 +1489,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C41" s="3">
         <v>1</v>
@@ -1501,15 +1504,15 @@
         <v>11.06</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
@@ -1524,12 +1527,12 @@
         <v>1.69</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
@@ -1544,15 +1547,15 @@
         <v>15.42</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C44" s="3">
         <v>1</v>
@@ -1572,7 +1575,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C45" s="3">
         <v>5</v>
@@ -1592,7 +1595,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C46" s="3">
         <v>5</v>
@@ -1607,6 +1610,43 @@
         <v>11.76</v>
       </c>
       <c r="G46" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" s="3">
+        <v>2</v>
+      </c>
+      <c r="F47" s="1">
+        <v>11.78</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="3">
+        <v>100</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
+        <v>99</v>
+      </c>
+      <c r="F48" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="G48" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1618,46 +1658,48 @@
     <hyperlink ref="A5" r:id="rId4" xr:uid="{ADAE3393-F93E-45A1-AEA2-8759FB728108}"/>
     <hyperlink ref="A6" r:id="rId5" xr:uid="{31669652-EDC7-4FB3-8474-05F259029E52}"/>
     <hyperlink ref="A7" r:id="rId6" xr:uid="{09B66535-5BE6-4839-BD51-A4F7FD4D6898}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{9BCD095B-47DC-410F-9079-F7EF1073AAB6}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{602A26C0-072C-4CA0-B060-8605A9A79C99}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{CB2F58B0-3E1A-45F1-9BAF-84747E9E2286}"/>
-    <hyperlink ref="A12" r:id="rId10" xr:uid="{3248FF67-9F07-4CAC-8A23-E7D040BAF240}"/>
-    <hyperlink ref="A13" r:id="rId11" xr:uid="{036623F6-4A17-4DC1-B412-5D2B9F531304}"/>
-    <hyperlink ref="A14" r:id="rId12" xr:uid="{FE7980E9-66C7-4203-A284-299B9289A69F}"/>
-    <hyperlink ref="A15" r:id="rId13" xr:uid="{919D209F-D950-4910-849B-5AB77A6C3FE8}"/>
-    <hyperlink ref="A16" r:id="rId14" xr:uid="{B39BD6B0-9D3E-4F4D-9289-008736E9AB9E}"/>
-    <hyperlink ref="A17" r:id="rId15" xr:uid="{DC2AB890-168C-4E32-A4B1-D4FE8EFB056E}"/>
-    <hyperlink ref="A18" r:id="rId16" xr:uid="{3B9AA3BB-A878-47F5-8FD7-E001F7473C4C}"/>
-    <hyperlink ref="A19" r:id="rId17" xr:uid="{71194D6C-4C2C-40AE-BA02-4EE66C79B901}"/>
-    <hyperlink ref="A20" r:id="rId18" xr:uid="{06D49833-6463-4404-A46B-44C35596620D}"/>
-    <hyperlink ref="A21" r:id="rId19" xr:uid="{49D42AB6-4BE9-4066-8807-9A44A8AE697C}"/>
-    <hyperlink ref="A22" r:id="rId20" xr:uid="{D39B49A4-0862-4B0C-A68D-D8A021F9D2A2}"/>
-    <hyperlink ref="A24" r:id="rId21" xr:uid="{CFEE09BC-B295-4BB1-A6E5-DC54B1C602CC}"/>
-    <hyperlink ref="A25" r:id="rId22" xr:uid="{D1AF1FD1-DBE3-4AF5-A0AF-E7534826D87A}"/>
-    <hyperlink ref="A26" r:id="rId23" xr:uid="{C84E2B92-5A19-4D83-8C00-11FF9D3EB587}"/>
-    <hyperlink ref="A30" r:id="rId24" xr:uid="{BEA5C90D-4828-4877-8CED-76D896634F61}"/>
-    <hyperlink ref="A32" r:id="rId25" xr:uid="{312B116C-2D5F-4265-9413-EA9A4EFC773E}"/>
-    <hyperlink ref="A33" r:id="rId26" xr:uid="{BBEFB0EB-6635-402F-8279-A218F7AAAA00}"/>
-    <hyperlink ref="A34" r:id="rId27" xr:uid="{6A4C2A30-E829-4BBF-AB3B-22342EB906B0}"/>
-    <hyperlink ref="A35" r:id="rId28" xr:uid="{2E46890A-5D0A-4A55-9352-0ED0800B2E7E}"/>
-    <hyperlink ref="A36" r:id="rId29" xr:uid="{6359A94C-E108-400B-9B0C-E90D5B3F3C1B}"/>
-    <hyperlink ref="A27" r:id="rId30" xr:uid="{64D620F9-BE29-4078-8FDB-01AADED4CD5A}"/>
-    <hyperlink ref="A11" r:id="rId31" xr:uid="{73E346AF-CF78-462D-A1B5-06E16522D199}"/>
-    <hyperlink ref="A29" r:id="rId32" xr:uid="{068F758C-56B5-4BE6-8457-882D40684EC8}"/>
-    <hyperlink ref="A23" r:id="rId33" xr:uid="{DD1952C6-DDB9-46AB-BAF6-438AD299B4B9}"/>
-    <hyperlink ref="A37" r:id="rId34" xr:uid="{8EDB4583-9C54-449A-B150-77F255495BD5}"/>
-    <hyperlink ref="A38" r:id="rId35" xr:uid="{F26BE873-0541-4AD7-B469-EEC4ECF1ACE8}"/>
-    <hyperlink ref="A39" r:id="rId36" xr:uid="{A56A6466-8646-4733-BAB4-237D1A4B7620}"/>
-    <hyperlink ref="A40" r:id="rId37" xr:uid="{081913BF-1751-47D6-B8AD-C966158B1155}"/>
-    <hyperlink ref="A28" r:id="rId38" display="Adafruit 858 Stepper Motor" xr:uid="{474E9ED2-9AFC-49D6-855D-64137217487B}"/>
-    <hyperlink ref="A41" r:id="rId39" xr:uid="{1F56827A-8EC4-4506-A806-69B5F684DE5C}"/>
-    <hyperlink ref="A42" r:id="rId40" xr:uid="{12164573-0FDC-4B10-A12A-CC40E343CC16}"/>
-    <hyperlink ref="A43" r:id="rId41" xr:uid="{820FF4A0-CDA2-495F-8E9D-9F47FAB7A271}"/>
-    <hyperlink ref="A44" r:id="rId42" xr:uid="{C3F4C230-2C94-4F28-852B-556D69F4D837}"/>
-    <hyperlink ref="A45" r:id="rId43" xr:uid="{8D69888B-2039-4A9C-973D-8028D4E1E97C}"/>
-    <hyperlink ref="A46" r:id="rId44" xr:uid="{D16355A9-735E-4FF6-8453-810E60FD4015}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{602A26C0-072C-4CA0-B060-8605A9A79C99}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{CB2F58B0-3E1A-45F1-9BAF-84747E9E2286}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{3248FF67-9F07-4CAC-8A23-E7D040BAF240}"/>
+    <hyperlink ref="A13" r:id="rId10" xr:uid="{036623F6-4A17-4DC1-B412-5D2B9F531304}"/>
+    <hyperlink ref="A14" r:id="rId11" xr:uid="{FE7980E9-66C7-4203-A284-299B9289A69F}"/>
+    <hyperlink ref="A15" r:id="rId12" xr:uid="{919D209F-D950-4910-849B-5AB77A6C3FE8}"/>
+    <hyperlink ref="A16" r:id="rId13" xr:uid="{B39BD6B0-9D3E-4F4D-9289-008736E9AB9E}"/>
+    <hyperlink ref="A17" r:id="rId14" xr:uid="{DC2AB890-168C-4E32-A4B1-D4FE8EFB056E}"/>
+    <hyperlink ref="A18" r:id="rId15" xr:uid="{3B9AA3BB-A878-47F5-8FD7-E001F7473C4C}"/>
+    <hyperlink ref="A19" r:id="rId16" xr:uid="{71194D6C-4C2C-40AE-BA02-4EE66C79B901}"/>
+    <hyperlink ref="A20" r:id="rId17" xr:uid="{06D49833-6463-4404-A46B-44C35596620D}"/>
+    <hyperlink ref="A21" r:id="rId18" xr:uid="{49D42AB6-4BE9-4066-8807-9A44A8AE697C}"/>
+    <hyperlink ref="A22" r:id="rId19" xr:uid="{D39B49A4-0862-4B0C-A68D-D8A021F9D2A2}"/>
+    <hyperlink ref="A24" r:id="rId20" xr:uid="{CFEE09BC-B295-4BB1-A6E5-DC54B1C602CC}"/>
+    <hyperlink ref="A25" r:id="rId21" xr:uid="{D1AF1FD1-DBE3-4AF5-A0AF-E7534826D87A}"/>
+    <hyperlink ref="A26" r:id="rId22" xr:uid="{C84E2B92-5A19-4D83-8C00-11FF9D3EB587}"/>
+    <hyperlink ref="A30" r:id="rId23" xr:uid="{BEA5C90D-4828-4877-8CED-76D896634F61}"/>
+    <hyperlink ref="A32" r:id="rId24" xr:uid="{312B116C-2D5F-4265-9413-EA9A4EFC773E}"/>
+    <hyperlink ref="A33" r:id="rId25" xr:uid="{BBEFB0EB-6635-402F-8279-A218F7AAAA00}"/>
+    <hyperlink ref="A34" r:id="rId26" xr:uid="{6A4C2A30-E829-4BBF-AB3B-22342EB906B0}"/>
+    <hyperlink ref="A35" r:id="rId27" xr:uid="{2E46890A-5D0A-4A55-9352-0ED0800B2E7E}"/>
+    <hyperlink ref="A36" r:id="rId28" xr:uid="{6359A94C-E108-400B-9B0C-E90D5B3F3C1B}"/>
+    <hyperlink ref="A27" r:id="rId29" xr:uid="{64D620F9-BE29-4078-8FDB-01AADED4CD5A}"/>
+    <hyperlink ref="A29" r:id="rId30" xr:uid="{068F758C-56B5-4BE6-8457-882D40684EC8}"/>
+    <hyperlink ref="A23" r:id="rId31" xr:uid="{DD1952C6-DDB9-46AB-BAF6-438AD299B4B9}"/>
+    <hyperlink ref="A37" r:id="rId32" xr:uid="{8EDB4583-9C54-449A-B150-77F255495BD5}"/>
+    <hyperlink ref="A38" r:id="rId33" xr:uid="{F26BE873-0541-4AD7-B469-EEC4ECF1ACE8}"/>
+    <hyperlink ref="A39" r:id="rId34" xr:uid="{A56A6466-8646-4733-BAB4-237D1A4B7620}"/>
+    <hyperlink ref="A40" r:id="rId35" xr:uid="{081913BF-1751-47D6-B8AD-C966158B1155}"/>
+    <hyperlink ref="A28" r:id="rId36" display="Adafruit 858 Stepper Motor" xr:uid="{474E9ED2-9AFC-49D6-855D-64137217487B}"/>
+    <hyperlink ref="A41" r:id="rId37" xr:uid="{1F56827A-8EC4-4506-A806-69B5F684DE5C}"/>
+    <hyperlink ref="A42" r:id="rId38" xr:uid="{12164573-0FDC-4B10-A12A-CC40E343CC16}"/>
+    <hyperlink ref="A43" r:id="rId39" xr:uid="{820FF4A0-CDA2-495F-8E9D-9F47FAB7A271}"/>
+    <hyperlink ref="A44" r:id="rId40" xr:uid="{C3F4C230-2C94-4F28-852B-556D69F4D837}"/>
+    <hyperlink ref="A45" r:id="rId41" xr:uid="{8D69888B-2039-4A9C-973D-8028D4E1E97C}"/>
+    <hyperlink ref="A46" r:id="rId42" xr:uid="{D16355A9-735E-4FF6-8453-810E60FD4015}"/>
+    <hyperlink ref="A47" r:id="rId43" xr:uid="{3BAF9296-1533-4F8F-A166-14A908B510E0}"/>
+    <hyperlink ref="A48" r:id="rId44" xr:uid="{02EA597A-AE68-4FCA-9F83-86A70357D802}"/>
+    <hyperlink ref="A8" r:id="rId45" xr:uid="{9BCD095B-47DC-410F-9079-F7EF1073AAB6}"/>
+    <hyperlink ref="A11" r:id="rId46" xr:uid="{76FFA5A7-6500-4CCF-9FA6-A74E10BB2226}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId45"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>